<commit_message>
Update self evaluation protocol
</commit_message>
<xml_diff>
--- a/documents/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/documents/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilian\Documents\GitHub\iBook\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -641,7 +641,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1137,11 +1139,12 @@
         <v>9</v>
       </c>
       <c r="C44" s="11">
-        <v>260</v>
+        <f>SUM(C11:C43) + 100</f>
+        <v>360</v>
       </c>
       <c r="D44" s="11">
-        <f>SUM(D11:D43)</f>
-        <v>270</v>
+        <f>SUM(D11:D43) + 100</f>
+        <v>370</v>
       </c>
       <c r="E44" s="1"/>
     </row>

</xml_diff>